<commit_message>
Revert "Merge branch 'main' of https://github.com/usckrc/BTG"
This reverts commit 0c11fb893d1f8bddb70bda6d1d690433409aad8d, reversing
changes made to 5b5806dd306e54025d9cdf822b285f67fd0804da.
</commit_message>
<xml_diff>
--- a/summer_2025_schedule/rt_projected_schedule.xlsx
+++ b/summer_2025_schedule/rt_projected_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive - University of Southern California\Github\BTG\summer_2025_schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sblanche/Desktop/GitHub/BTG /summer_2025_schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D05A288-97EC-4342-8D36-28A4C29B1B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063B36E4-ABE7-3340-8B01-2E69BA57B853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{709B4272-95D4-4CE2-9E15-1F20C641EF30}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="14460" windowHeight="16860" xr2:uid="{709B4272-95D4-4CE2-9E15-1F20C641EF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Week 1</t>
   </si>
@@ -128,6 +128,9 @@
     <t>Subject</t>
   </si>
   <si>
+    <t>Barron and Boulpaep Ch. 32</t>
+  </si>
+  <si>
     <t>Barron and Boulpaep Ch. 33</t>
   </si>
   <si>
@@ -143,6 +146,9 @@
     <t>Barron and Boulpaep Ch. 37</t>
   </si>
   <si>
+    <t>Barron and Boulpaep Ch. 39</t>
+  </si>
+  <si>
     <t>Transport of Sodium and Chloride</t>
   </si>
   <si>
@@ -179,56 +185,50 @@
     <t xml:space="preserve">scRNAseq analysis of human biopsies for Chronic Kidney Disease </t>
   </si>
   <si>
-    <t>Barron and Boulpaep Ch. 38</t>
-  </si>
-  <si>
-    <t>Barron and Boulpaep Ch. 40</t>
-  </si>
-  <si>
-    <t>Ten simple rules for structuring papers.pdf</t>
-  </si>
-  <si>
-    <t>Ten simple rules for reading a scientific paper.pdf</t>
-  </si>
-  <si>
-    <t>Ten Simple Rules for Reproducible Computational Research.pdf</t>
-  </si>
-  <si>
-    <t>Ten simple rules for biologists learning to program.pdf</t>
-  </si>
-  <si>
-    <t>Ten Simple Rules for Better Figures.pdf</t>
-  </si>
-  <si>
-    <t>Ten simple rules for teaching an introduction to R.pdf</t>
-  </si>
-  <si>
-    <t>Ten Simple Rules for Making Good Oral Presentations.pdf</t>
-  </si>
-  <si>
-    <t>Pippetting</t>
-  </si>
-  <si>
-    <t>DNA Digest</t>
-  </si>
-  <si>
-    <t>qPCR</t>
-  </si>
-  <si>
-    <t>Mouse Tagging and Tailing</t>
-  </si>
-  <si>
-    <t>Mouse Perfusion</t>
-  </si>
-  <si>
-    <t>ELISA Albuwell</t>
+    <t>Psuedobulk</t>
+  </si>
+  <si>
+    <t>Education Website - ROC 1</t>
+  </si>
+  <si>
+    <t>Intro to R &amp; Setup</t>
+  </si>
+  <si>
+    <t>Data Visualization &amp; Interpretation</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Manuscript Writing</t>
+  </si>
+  <si>
+    <t>Uploading files from GEO and other Seurat Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rmarkdown &amp; the whole kidney </t>
+  </si>
+  <si>
+    <t>Ddataset integration</t>
+  </si>
+  <si>
+    <t>Week 3 Materials_for_Seurat_v5 + HW 3</t>
+  </si>
+  <si>
+    <t>ROC 4 + HW 2</t>
+  </si>
+  <si>
+    <t>ROC 2 + HW 1</t>
+  </si>
+  <si>
+    <t>AL-Pseudobulk-Materials + HW 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +240,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -604,26 +610,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96431D7-ED8A-48B0-9E19-0BDA6085CDA8}">
-  <dimension ref="B1:L34"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="5" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1640625" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
@@ -645,7 +651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
@@ -667,13 +673,19 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
@@ -681,16 +693,22 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
@@ -698,189 +716,157 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
         <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
-        <v>50</v>
-      </c>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
-        <v>61</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 INTERNAL</oddFooter>

</xml_diff>

<commit_message>
Reapply "Merge branch 'main' of https://github.com/usckrc/BTG"
This reverts commit 4d20f7cd93e7c4cb426a4c211d064259a59b8b1f.
</commit_message>
<xml_diff>
--- a/summer_2025_schedule/rt_projected_schedule.xlsx
+++ b/summer_2025_schedule/rt_projected_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sblanche/Desktop/GitHub/BTG /summer_2025_schedule/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive - University of Southern California\Github\BTG\summer_2025_schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063B36E4-ABE7-3340-8B01-2E69BA57B853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D05A288-97EC-4342-8D36-28A4C29B1B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="14460" windowHeight="16860" xr2:uid="{709B4272-95D4-4CE2-9E15-1F20C641EF30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{709B4272-95D4-4CE2-9E15-1F20C641EF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>Week 1</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Barron and Boulpaep Ch. 32</t>
-  </si>
-  <si>
     <t>Barron and Boulpaep Ch. 33</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>Barron and Boulpaep Ch. 37</t>
   </si>
   <si>
-    <t>Barron and Boulpaep Ch. 39</t>
-  </si>
-  <si>
     <t>Transport of Sodium and Chloride</t>
   </si>
   <si>
@@ -185,50 +179,56 @@
     <t xml:space="preserve">scRNAseq analysis of human biopsies for Chronic Kidney Disease </t>
   </si>
   <si>
-    <t>Psuedobulk</t>
-  </si>
-  <si>
-    <t>Education Website - ROC 1</t>
-  </si>
-  <si>
-    <t>Intro to R &amp; Setup</t>
-  </si>
-  <si>
-    <t>Data Visualization &amp; Interpretation</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Manuscript Writing</t>
-  </si>
-  <si>
-    <t>Uploading files from GEO and other Seurat Functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rmarkdown &amp; the whole kidney </t>
-  </si>
-  <si>
-    <t>Ddataset integration</t>
-  </si>
-  <si>
-    <t>Week 3 Materials_for_Seurat_v5 + HW 3</t>
-  </si>
-  <si>
-    <t>ROC 4 + HW 2</t>
-  </si>
-  <si>
-    <t>ROC 2 + HW 1</t>
-  </si>
-  <si>
-    <t>AL-Pseudobulk-Materials + HW 4</t>
+    <t>Barron and Boulpaep Ch. 38</t>
+  </si>
+  <si>
+    <t>Barron and Boulpaep Ch. 40</t>
+  </si>
+  <si>
+    <t>Ten simple rules for structuring papers.pdf</t>
+  </si>
+  <si>
+    <t>Ten simple rules for reading a scientific paper.pdf</t>
+  </si>
+  <si>
+    <t>Ten Simple Rules for Reproducible Computational Research.pdf</t>
+  </si>
+  <si>
+    <t>Ten simple rules for biologists learning to program.pdf</t>
+  </si>
+  <si>
+    <t>Ten Simple Rules for Better Figures.pdf</t>
+  </si>
+  <si>
+    <t>Ten simple rules for teaching an introduction to R.pdf</t>
+  </si>
+  <si>
+    <t>Ten Simple Rules for Making Good Oral Presentations.pdf</t>
+  </si>
+  <si>
+    <t>Pippetting</t>
+  </si>
+  <si>
+    <t>DNA Digest</t>
+  </si>
+  <si>
+    <t>qPCR</t>
+  </si>
+  <si>
+    <t>Mouse Tagging and Tailing</t>
+  </si>
+  <si>
+    <t>Mouse Perfusion</t>
+  </si>
+  <si>
+    <t>ELISA Albuwell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,12 +240,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -610,26 +604,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96431D7-ED8A-48B0-9E19-0BDA6085CDA8}">
-  <dimension ref="B1:L17"/>
+  <dimension ref="B1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1640625" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
@@ -651,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
@@ -673,19 +667,13 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
@@ -693,22 +681,16 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
@@ -716,157 +698,189 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" t="s">
-        <v>59</v>
-      </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s">
-        <v>58</v>
-      </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
         <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
       <c r="J17" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 INTERNAL</oddFooter>

</xml_diff>